<commit_message>
write results and return resuts as excel to client
</commit_message>
<xml_diff>
--- a/ExcelDemoAPI/Files/WeatherExcel.xlsx
+++ b/ExcelDemoAPI/Files/WeatherExcel.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -29,13 +29,13 @@
     <t>11/6/2023</t>
   </si>
   <si>
-    <t>Warm</t>
+    <t>Freezing</t>
   </si>
   <si>
     <t>11/7/2023</t>
   </si>
   <si>
-    <t>Bracing</t>
+    <t>Sweltering</t>
   </si>
   <si>
     <t>11/8/2023</t>
@@ -47,10 +47,13 @@
     <t>11/9/2023</t>
   </si>
   <si>
+    <t>Balmy</t>
+  </si>
+  <si>
     <t>11/10/2023</t>
   </si>
   <si>
-    <t>Freezing</t>
+    <t>Mild</t>
   </si>
 </sst>
 </file>
@@ -105,7 +108,7 @@
     <col min="1" max="1" width="11.115262985229492" customWidth="1"/>
     <col min="2" max="2" width="13.375214576721191" customWidth="1"/>
     <col min="3" max="3" width="13.215616226196289" customWidth="1"/>
-    <col min="4" max="4" width="9.182692527770996" customWidth="1"/>
+    <col min="4" max="4" width="9.9960298538208" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -127,10 +130,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="0">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C2" s="0">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>5</v>
@@ -141,10 +144,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="0">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0">
-        <v>116</v>
+        <v>84</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>7</v>
@@ -155,10 +158,10 @@
         <v>8</v>
       </c>
       <c r="B4" s="0">
-        <v>-18</v>
+        <v>34</v>
       </c>
       <c r="C4" s="0">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>9</v>
@@ -169,27 +172,27 @@
         <v>10</v>
       </c>
       <c r="B5" s="0">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="C5" s="0">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C6" s="0">
-        <v>98</v>
+        <v>44</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>